<commit_message>
TRD list info start
</commit_message>
<xml_diff>
--- a/docs/WIP/TaskRiskDecision.xlsx
+++ b/docs/WIP/TaskRiskDecision.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="TaskList" sheetId="1" r:id="rId1"/>
@@ -14,6 +14,77 @@
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>owner</t>
+  </si>
+  <si>
+    <t>status</t>
+  </si>
+  <si>
+    <t>deadline</t>
+  </si>
+  <si>
+    <t>updates</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>Risk event</t>
+  </si>
+  <si>
+    <t>Probability</t>
+  </si>
+  <si>
+    <t>Impact</t>
+  </si>
+  <si>
+    <t>Priority</t>
+  </si>
+  <si>
+    <t>State</t>
+  </si>
+  <si>
+    <t>open/closed</t>
+  </si>
+  <si>
+    <t>Risk area</t>
+  </si>
+  <si>
+    <t>global…</t>
+  </si>
+  <si>
+    <t>Proposed solution</t>
+  </si>
+  <si>
+    <t>Response</t>
+  </si>
+  <si>
+    <t>Areas impacted</t>
+  </si>
+  <si>
+    <t>time</t>
+  </si>
+  <si>
+    <t>cost</t>
+  </si>
+  <si>
+    <t>scope</t>
+  </si>
+  <si>
+    <t>quality</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -47,8 +118,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -353,54 +428,159 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="C3:F6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+    </row>
+    <row r="6" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E6" s="1"/>
+      <c r="F6" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="C5:F5"/>
+    <mergeCell ref="D6:E6"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:N3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="G1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H2" t="s">
+        <v>12</v>
+      </c>
+      <c r="I2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="K3" t="s">
+        <v>17</v>
+      </c>
+      <c r="L3" t="s">
+        <v>18</v>
+      </c>
+      <c r="M3" t="s">
+        <v>19</v>
+      </c>
+      <c r="N3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+      <selection activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Revert "Merge branch 'master' of gitlab.fel.cvut.cz:B162_B6B36RSP/102_CASA"
This reverts commit cd1f352157816ee1b808e47c2aa91b4f2feeb2cb
</commit_message>
<xml_diff>
--- a/docs/WIP/TaskRiskDecision.xlsx
+++ b/docs/WIP/TaskRiskDecision.xlsx
@@ -10,91 +10,10 @@
     <sheet name="TaskList" sheetId="1" r:id="rId1"/>
     <sheet name="RiskList" sheetId="2" r:id="rId2"/>
     <sheet name="KeyDecisions" sheetId="3" r:id="rId3"/>
-    <sheet name="ChangeRequests" sheetId="5" r:id="rId4"/>
-    <sheet name="LessonsLearned" sheetId="4" r:id="rId5"/>
+    <sheet name="LessonsLearned" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
-</file>
-
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="25">
-  <si>
-    <t>description</t>
-  </si>
-  <si>
-    <t>owner</t>
-  </si>
-  <si>
-    <t>status</t>
-  </si>
-  <si>
-    <t>deadline</t>
-  </si>
-  <si>
-    <t>updates</t>
-  </si>
-  <si>
-    <t>date</t>
-  </si>
-  <si>
-    <t>Risk event</t>
-  </si>
-  <si>
-    <t>Probability</t>
-  </si>
-  <si>
-    <t>Impact</t>
-  </si>
-  <si>
-    <t>Priority</t>
-  </si>
-  <si>
-    <t>State</t>
-  </si>
-  <si>
-    <t>open/closed</t>
-  </si>
-  <si>
-    <t>Risk area</t>
-  </si>
-  <si>
-    <t>global…</t>
-  </si>
-  <si>
-    <t>Proposed solution</t>
-  </si>
-  <si>
-    <t>Response</t>
-  </si>
-  <si>
-    <t>Areas impacted</t>
-  </si>
-  <si>
-    <t>time</t>
-  </si>
-  <si>
-    <t>cost</t>
-  </si>
-  <si>
-    <t>scope</t>
-  </si>
-  <si>
-    <t>quality</t>
-  </si>
-  <si>
-    <t>ID</t>
-  </si>
-  <si>
-    <t>Description</t>
-  </si>
-  <si>
-    <t>Scope</t>
-  </si>
-  <si>
-    <t>Agreed?</t>
-  </si>
-</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -128,12 +47,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -438,188 +353,54 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C3:F6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="3" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E3" t="s">
-        <v>3</v>
-      </c>
-      <c r="F3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C5" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-    </row>
-    <row r="6" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C6" t="s">
-        <v>5</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="E6" s="2"/>
-      <c r="F6" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="C5:F5"/>
-    <mergeCell ref="D6:E6"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:N3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="G1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G2" t="s">
-        <v>10</v>
-      </c>
-      <c r="H2" t="s">
-        <v>12</v>
-      </c>
-      <c r="I2" t="s">
-        <v>14</v>
-      </c>
-      <c r="J2" t="s">
-        <v>15</v>
-      </c>
-      <c r="K2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="K3" t="s">
-        <v>17</v>
-      </c>
-      <c r="L3" t="s">
-        <v>18</v>
-      </c>
-      <c r="M3" t="s">
-        <v>19</v>
-      </c>
-      <c r="N3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:E2"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D2" t="s">
-        <v>23</v>
-      </c>
-      <c r="E2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M4" sqref="M4"/>
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>